<commit_message>
update for new version 2024
</commit_message>
<xml_diff>
--- a/Performance.xlsx
+++ b/Performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\eclipse-workspace-DL\DeepCry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4641D809-97B4-4D57-8C13-293C6276A1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3894E5-DDF6-466F-9B33-F2EE17E2F18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-160" yWindow="3120" windowWidth="28800" windowHeight="15450" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -21,22 +21,22 @@
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Performance!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Performance!$O$2:$O$10</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Performance!$P$2:$P$10</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Performance!$Q$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Performance!$W$2:$W$10</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">Performance!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Performance!$Q$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Performance!$Q$2:$Q$10</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Performance!$R$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Performance!$R$2:$R$10</definedName>
     <definedName name="_xlchart.v1.14" hidden="1">Performance!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Performance!$W$1</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Performance!$W$2:$W$10</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Performance!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Performance!$R$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Performance!$R$2:$R$10</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Performance!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Performance!$C$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Performance!$C$2:$C$10</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Performance!$C$1</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Performance!$C$2:$C$10</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Performance!$Q$2:$Q$10</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Performance!$B$2:$B$10</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Performance!$P$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Performance!$P$2:$P$10</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Performance!$B$2:$B$10</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Performance!$O$2:$O$10</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">Performance!$B$2:$B$10</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Performance!$P$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Performance!$W$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -448,7 +448,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>SNR (dB) vs</a:t>
+              <a:t>SNR vs</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="it-IT" baseline="0"/>
@@ -2270,10 +2270,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2346,10 +2346,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.10</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2387,7 +2387,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{69B320A9-5D37-46E1-B9C8-2F719F17411D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.9</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>precision</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2428,10 +2428,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2469,7 +2469,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{69B320A9-5D37-46E1-B9C8-2F719F17411D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>recall</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2510,10 +2510,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2551,7 +2551,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{69B320A9-5D37-46E1-B9C8-2F719F17411D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.3</cx:f>
+              <cx:f>_xlchart.v1.12</cx:f>
               <cx:v>f1</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2592,10 +2592,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.16</cx:f>
+        <cx:f>_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2633,7 +2633,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{69B320A9-5D37-46E1-B9C8-2F719F17411D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.15</cx:f>
+              <cx:f>_xlchart.v1.9</cx:f>
               <cx:v>kappa</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2674,10 +2674,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.14</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.16</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2715,7 +2715,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{69B320A9-5D37-46E1-B9C8-2F719F17411D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:f>_xlchart.v1.15</cx:f>
               <cx:v>snr</cx:v>
             </cx:txData>
           </cx:tx>
@@ -7572,8 +7572,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2514600" y="4450896"/>
-              <a:ext cx="4276726" cy="3187699"/>
+              <a:off x="2514600" y="4603296"/>
+              <a:ext cx="3981451" cy="3295649"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7650,8 +7650,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6934200" y="4469946"/>
-              <a:ext cx="4756151" cy="3187699"/>
+              <a:off x="6638925" y="4622346"/>
+              <a:ext cx="4724401" cy="3295649"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7728,8 +7728,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="11861800" y="4479471"/>
-              <a:ext cx="4876801" cy="3187699"/>
+              <a:off x="11534775" y="4631871"/>
+              <a:ext cx="4762501" cy="3295649"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7806,8 +7806,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2496911" y="7728403"/>
-              <a:ext cx="4297136" cy="3181349"/>
+              <a:off x="2496911" y="7988753"/>
+              <a:ext cx="4001861" cy="3295649"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7884,8 +7884,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6908347" y="7727042"/>
-              <a:ext cx="4756151" cy="3181349"/>
+              <a:off x="6613072" y="7987392"/>
+              <a:ext cx="4724401" cy="3295649"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7962,8 +7962,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="11848194" y="7727043"/>
-              <a:ext cx="4856390" cy="3181349"/>
+              <a:off x="11521169" y="7987393"/>
+              <a:ext cx="4742090" cy="3295649"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8383,27 +8383,27 @@
       <selection activeCell="AD1" sqref="AD1:AD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="74.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.7265625" customWidth="1"/>
-    <col min="27" max="27" width="19.26953125" customWidth="1"/>
-    <col min="28" max="28" width="22.54296875" customWidth="1"/>
-    <col min="29" max="29" width="26.1796875" customWidth="1"/>
-    <col min="30" max="30" width="50.7265625" style="4" customWidth="1"/>
-    <col min="31" max="31" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="60.7265625" customWidth="1"/>
+    <col min="1" max="1" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.7109375" customWidth="1"/>
+    <col min="27" max="27" width="19.28515625" customWidth="1"/>
+    <col min="28" max="28" width="22.5703125" customWidth="1"/>
+    <col min="29" max="29" width="26.140625" customWidth="1"/>
+    <col min="30" max="30" width="50.7109375" style="4" customWidth="1"/>
+    <col min="31" max="31" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8501,7 +8501,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -8602,7 +8602,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -8703,7 +8703,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -8804,7 +8804,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -8905,7 +8905,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -9006,7 +9006,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -9107,7 +9107,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -9208,7 +9208,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -9309,7 +9309,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -9422,7 +9422,7 @@
       <c r="W11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
@@ -9524,7 +9524,7 @@
         <v>16.333333333333332</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>71</v>
       </c>
@@ -9578,7 +9578,7 @@
         <v>8.4666666666666668</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>73</v>
       </c>
@@ -9632,7 +9632,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>72</v>
       </c>
@@ -9701,17 +9701,17 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.1796875" style="5"/>
-    <col min="6" max="7" width="9.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7265625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="5"/>
+    <col min="6" max="7" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>40</v>
       </c>
@@ -9743,7 +9743,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>71</v>
       </c>
@@ -9775,7 +9775,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>71</v>
       </c>
@@ -9807,7 +9807,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>71</v>
       </c>
@@ -9839,7 +9839,7 @@
         <v>7.5166666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>73</v>
       </c>
@@ -9871,7 +9871,7 @@
         <v>2.5333333333333332</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>73</v>
       </c>
@@ -9903,7 +9903,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>73</v>
       </c>
@@ -9935,7 +9935,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>73</v>
       </c>
@@ -9967,7 +9967,7 @@
         <v>0.8833333333333333</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>72</v>
       </c>
@@ -9999,7 +9999,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
@@ -10031,7 +10031,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -10039,7 +10039,7 @@
       <c r="G11" s="7"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>41</v>
       </c>
@@ -10071,7 +10071,7 @@
         <v>16.333333333333332</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>76</v>
       </c>
@@ -10104,7 +10104,7 @@
         <v>8.4666666666666668</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>77</v>
       </c>
@@ -10137,7 +10137,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>78</v>
       </c>
@@ -10181,16 +10181,16 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>87</v>
       </c>
@@ -10210,7 +10210,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3.12869271030545</v>
       </c>
@@ -10230,7 +10230,7 @@
         <v>0.73864429404214305</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4.4048959473515197</v>
       </c>
@@ -10250,7 +10250,7 @@
         <v>0.139286312738678</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>5.0523168087946901</v>
       </c>
@@ -10270,7 +10270,7 @@
         <v>0.267446825708056</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>6.0375992830992899</v>
       </c>
@@ -10290,7 +10290,7 @@
         <v>8.4319984469194101E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>9.4416905218884395</v>
       </c>
@@ -10310,7 +10310,7 @@
         <v>0.79225372302574004</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>13.662433206723801</v>
       </c>
@@ -10330,7 +10330,7 @@
         <v>0.480592436580282</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>16.706388264192899</v>
       </c>
@@ -10350,7 +10350,7 @@
         <v>0.60111202179827705</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>16.860605159999999</v>
       </c>
@@ -10370,7 +10370,7 @@
         <v>0.312208649</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>20.006339908803401</v>
       </c>
@@ -10408,16 +10408,16 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.26953125" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -10431,7 +10431,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -10445,7 +10445,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -10459,7 +10459,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -10473,7 +10473,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -10487,7 +10487,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -10501,7 +10501,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -10515,7 +10515,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -10529,7 +10529,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -10543,7 +10543,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>59</v>
       </c>
@@ -10557,7 +10557,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -10574,7 +10574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -10591,7 +10591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -10608,7 +10608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>74</v>
       </c>
@@ -10616,7 +10616,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -10627,7 +10627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>73</v>
       </c>
@@ -10638,7 +10638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -10663,52 +10663,52 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -10717,7 +10717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>

</xml_diff>